<commit_message>
Add GDPR compliant banner
</commit_message>
<xml_diff>
--- a/supplementary-material/inputs/instruments.xlsx
+++ b/supplementary-material/inputs/instruments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtay0016/dev/youth-homelessness-review/supplementary-material/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA7FEA3-1944-314D-89BF-7AE14582CA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F328130F-C00B-2F4D-8768-9C877526BF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{FE8D09C8-B55D-7349-9A3F-18ECAE9B2E78}"/>
   </bookViews>
@@ -254,7 +254,7 @@
     <t>Evidence of validation among population with complex needs identified</t>
   </si>
   <si>
-    <t>Evidence of validation for homeless youth population identified'</t>
+    <t>Evidence of validation for homeless youth population identified</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>